<commit_message>
Union All oraz Merge
</commit_message>
<xml_diff>
--- a/Pliki/Plik_testowy.xlsx
+++ b/Pliki/Plik_testowy.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>test1</t>
   </si>
@@ -427,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,4 +588,173 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7866</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>